<commit_message>
chore(inputs): rename to flat format Inputs/<Type>/YYYY_MM_<type>.xlsx and flatten directory structure
</commit_message>
<xml_diff>
--- a/Inputs/Deskcount/2025_08_deskcount.xlsx
+++ b/Inputs/Deskcount/2025_08_deskcount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greystar365.sharepoint.com/sites/CorporateOfficeStrategy/Shared Documents/General/Occupancy Data/Dashboard/Inputs/Deskcount/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_E35161E09DDAB7BB5CD1F6181239E262265FDBF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763CA094-D4C6-41A6-B548-8F2564FD3A97}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="11_E35161E09DDAB7BB5CD1F6181239E262265FDBF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBF3D592-375D-413E-963F-5C2A8A7FF3AC}"/>
   <bookViews>
     <workbookView xWindow="59535" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,15 +47,24 @@
     <t>Deskcount</t>
   </si>
   <si>
+    <t>RSF</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
+    <t>Include in Occupancy Calculation</t>
+  </si>
+  <si>
     <t>Albuquerque</t>
   </si>
   <si>
     <t>6565 Americas Parkway NE, suite 320</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Arlington</t>
   </si>
   <si>
@@ -95,15 +104,33 @@
     <t>Charlotte</t>
   </si>
   <si>
+    <t>2151 Hawkins Street</t>
+  </si>
+  <si>
     <t>Chicago</t>
   </si>
   <si>
     <t>311 South Wacker Drive</t>
   </si>
   <si>
+    <t>Dallas - Cypress Waters</t>
+  </si>
+  <si>
+    <t>8840 Cypress Waters Blvd</t>
+  </si>
+  <si>
+    <t>Dallas - Southlake</t>
+  </si>
+  <si>
+    <t>Granite Place Two at Southlake Town Square</t>
+  </si>
+  <si>
     <t>Escondido</t>
   </si>
   <si>
+    <t>960 Canterbury Place (suite 100 &amp; 220)</t>
+  </si>
+  <si>
     <t>Eugene</t>
   </si>
   <si>
@@ -228,6 +255,9 @@
   </si>
   <si>
     <t>800 Fifth Avenue</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Solana Beach</t>
@@ -264,6 +294,9 @@
     <t>Madrid</t>
   </si>
   <si>
+    <t>Torre Europa, Paseo Castellana 95</t>
+  </si>
+  <si>
     <t>Melbourne</t>
   </si>
   <si>
@@ -273,6 +306,9 @@
     <t>Mohali</t>
   </si>
   <si>
+    <t>CP-67, Site no 252, Sector 67, 4th, 5th. 6th, and 10th Floor</t>
+  </si>
+  <si>
     <t>Paris</t>
   </si>
   <si>
@@ -294,9 +330,15 @@
     <t>Singapore</t>
   </si>
   <si>
+    <t>2 Central Boulevard, #14-04A</t>
+  </si>
+  <si>
     <t>Sydney</t>
   </si>
   <si>
+    <t>39 Martin Place, Sydney</t>
+  </si>
+  <si>
     <t>The Hague</t>
   </si>
   <si>
@@ -315,58 +357,16 @@
     <t>827 19th Ave S, Suite 930</t>
   </si>
   <si>
-    <t>Include in Occupancy Calculation</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>RSF</t>
-  </si>
-  <si>
-    <t>Torre Europa, Paseo Castellana 95</t>
-  </si>
-  <si>
     <t>Shanghai</t>
   </si>
   <si>
     <t>No.669 Xinzha Road, One Museum, Jingan District</t>
   </si>
   <si>
-    <t>39 Martin Place, Sydney</t>
-  </si>
-  <si>
-    <t>Dallas - Cypress Waters</t>
-  </si>
-  <si>
-    <t>8840 Cypress Waters Blvd</t>
-  </si>
-  <si>
-    <t>Dallas - Southlake</t>
-  </si>
-  <si>
-    <t>Granite Place Two at Southlake Town Square</t>
-  </si>
-  <si>
-    <t>CP-67, Site no 252, Sector 67, 4th, 5th. 6th, and 10th Floor</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>960 Canterbury Place (suite 100 &amp; 220)</t>
-  </si>
-  <si>
-    <t>2151 Hawkins Street</t>
-  </si>
-  <si>
     <t>Seoul</t>
   </si>
   <si>
     <t>769 Magok-dong, Gangseo-gu</t>
-  </si>
-  <si>
-    <t>2 Central Boulevard, #14-04A</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,16 +817,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="43.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,21 +837,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6">
         <v>10</v>
@@ -860,18 +860,18 @@
         <v>2589</v>
       </c>
       <c r="E2" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="7">
         <v>37</v>
@@ -880,18 +880,18 @@
         <v>10166</v>
       </c>
       <c r="E3" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7">
         <v>58</v>
@@ -900,18 +900,18 @@
         <v>24836</v>
       </c>
       <c r="E4" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7">
         <v>51</v>
@@ -920,18 +920,18 @@
         <v>18328</v>
       </c>
       <c r="E5" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29.1">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7">
         <v>24</v>
@@ -940,18 +940,18 @@
         <v>3726</v>
       </c>
       <c r="E6" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7">
         <v>35</v>
@@ -960,18 +960,18 @@
         <v>6505</v>
       </c>
       <c r="E7" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
         <v>367</v>
@@ -980,18 +980,18 @@
         <v>69149</v>
       </c>
       <c r="E8" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="C9" s="7">
         <v>40</v>
@@ -1000,18 +1000,18 @@
         <v>7512</v>
       </c>
       <c r="E9" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C10" s="7">
         <v>45</v>
@@ -1020,18 +1020,18 @@
         <v>8070</v>
       </c>
       <c r="E10" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="C11" s="7">
         <v>79</v>
@@ -1040,18 +1040,18 @@
         <v>37171</v>
       </c>
       <c r="E11" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C12" s="7">
         <v>60</v>
@@ -1060,18 +1060,18 @@
         <v>14753</v>
       </c>
       <c r="E12" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7">
         <v>18</v>
@@ -1080,18 +1080,18 @@
         <v>4835</v>
       </c>
       <c r="E13" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C14" s="7">
         <v>2</v>
@@ -1100,18 +1100,18 @@
         <v>533</v>
       </c>
       <c r="E14" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7">
         <v>31</v>
@@ -1120,18 +1120,18 @@
         <v>9065</v>
       </c>
       <c r="E15" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C16" s="7">
         <v>37</v>
@@ -1140,18 +1140,18 @@
         <v>8444</v>
       </c>
       <c r="E16" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C17" s="7">
         <v>56</v>
@@ -1160,18 +1160,18 @@
         <v>22527</v>
       </c>
       <c r="E17" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7">
         <v>12</v>
@@ -1180,18 +1180,18 @@
         <v>3173</v>
       </c>
       <c r="E18" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C19" s="7">
         <v>8</v>
@@ -1200,18 +1200,18 @@
         <v>2506</v>
       </c>
       <c r="E19" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1220,18 +1220,18 @@
         <v>3204</v>
       </c>
       <c r="E20" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C21" s="7">
         <v>126</v>
@@ -1240,18 +1240,18 @@
         <v>26981</v>
       </c>
       <c r="E21" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7">
         <v>12</v>
@@ -1260,18 +1260,18 @@
         <v>3410</v>
       </c>
       <c r="E22" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C23" s="7">
         <v>24</v>
@@ -1280,18 +1280,18 @@
         <v>8936</v>
       </c>
       <c r="E23" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C24" s="7">
         <v>57</v>
@@ -1300,18 +1300,18 @@
         <v>14624</v>
       </c>
       <c r="E24" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C25" s="7">
         <v>20</v>
@@ -1320,18 +1320,18 @@
         <v>4321</v>
       </c>
       <c r="E25" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C26" s="7">
         <v>15</v>
@@ -1340,18 +1340,18 @@
         <v>3990</v>
       </c>
       <c r="E26" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C27" s="7">
         <v>115</v>
@@ -1360,18 +1360,18 @@
         <v>27498</v>
       </c>
       <c r="E27" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7">
         <v>38</v>
@@ -1380,18 +1380,18 @@
         <v>7794</v>
       </c>
       <c r="E28" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C29" s="7">
         <v>24</v>
@@ -1400,18 +1400,18 @@
         <v>5500</v>
       </c>
       <c r="E29" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C30" s="7">
         <v>15</v>
@@ -1420,18 +1420,18 @@
         <v>3426</v>
       </c>
       <c r="E30" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C31" s="7">
         <v>20</v>
@@ -1440,18 +1440,18 @@
         <v>6027</v>
       </c>
       <c r="E31" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C32" s="7">
         <v>59</v>
@@ -1460,18 +1460,18 @@
         <v>9154</v>
       </c>
       <c r="E32" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C33" s="7">
         <v>12</v>
@@ -1480,18 +1480,18 @@
         <v>2945</v>
       </c>
       <c r="E33" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C34" s="7">
         <v>151</v>
@@ -1500,18 +1500,18 @@
         <v>25567</v>
       </c>
       <c r="E34" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C35" s="7">
         <v>14</v>
@@ -1520,18 +1520,18 @@
         <v>3809</v>
       </c>
       <c r="E35" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.5">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C36" s="7">
         <v>30</v>
@@ -1540,18 +1540,18 @@
         <v>6152</v>
       </c>
       <c r="E36" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C37" s="7">
         <v>8</v>
@@ -1560,18 +1560,18 @@
         <v>2098</v>
       </c>
       <c r="E37" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C38" s="7">
         <v>20</v>
@@ -1580,18 +1580,18 @@
         <v>3552</v>
       </c>
       <c r="E38" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29.1">
       <c r="A39" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C39" s="7">
         <v>186</v>
@@ -1600,18 +1600,18 @@
         <v>23138</v>
       </c>
       <c r="E39" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C40" s="7">
         <v>61</v>
@@ -1620,18 +1620,18 @@
         <v>8369</v>
       </c>
       <c r="E40" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C41" s="7">
         <v>32</v>
@@ -1640,18 +1640,18 @@
         <v>3509</v>
       </c>
       <c r="E41" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="29.1">
       <c r="A42" s="3" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C42" s="7">
         <v>561</v>
@@ -1660,18 +1660,18 @@
         <v>95392</v>
       </c>
       <c r="E42" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="29.1">
       <c r="A43" s="3" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C43" s="7">
         <v>44</v>
@@ -1680,18 +1680,18 @@
         <v>6490</v>
       </c>
       <c r="E43" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="29.1">
+      <c r="A44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="C44" s="7">
         <v>15</v>
@@ -1700,18 +1700,18 @@
         <v>2869</v>
       </c>
       <c r="E44" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C45" s="7">
         <v>27</v>
@@ -1720,18 +1720,18 @@
         <v>1798</v>
       </c>
       <c r="E45" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C46" s="7">
         <v>28</v>
@@ -1740,18 +1740,18 @@
         <v>2440</v>
       </c>
       <c r="E46" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C47" s="7">
         <v>48</v>
@@ -1760,18 +1760,18 @@
         <v>7858</v>
       </c>
       <c r="E47" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="3" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C48" s="7">
         <v>46</v>
@@ -1780,18 +1780,18 @@
         <v>6415</v>
       </c>
       <c r="E48" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29.1">
       <c r="A49" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C49" s="7">
         <v>20</v>
@@ -1800,18 +1800,18 @@
         <v>3000</v>
       </c>
       <c r="E49" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="3" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C50" s="7">
         <v>18</v>
@@ -1820,18 +1820,18 @@
         <v>5356</v>
       </c>
       <c r="E50" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C51" s="7">
         <v>20</v>
@@ -1840,18 +1840,18 @@
         <v>4815</v>
       </c>
       <c r="E51" s="8">
-        <v>45839</v>
+        <v>45870</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C52" s="7">
         <v>9</v>
@@ -1859,8 +1859,11 @@
       <c r="D52" s="7">
         <v>4389</v>
       </c>
+      <c r="E52" s="8">
+        <v>45870</v>
+      </c>
       <c r="F52" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1869,6 +1872,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="247b3ed0-617a-4d1d-b8bd-a66944492619" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="334de605-b0fc-4c39-b9f0-ad19cf79a3ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012DDEC86E47B0D488EDE8526C5FE0957" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bf1f00915b321be1014b44a0a0242ec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="334de605-b0fc-4c39-b9f0-ad19cf79a3ca" xmlns:ns3="247b3ed0-617a-4d1d-b8bd-a66944492619" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a82e13236a0edc0785210399e43caf" ns2:_="" ns3:_="">
     <xsd:import namespace="334de605-b0fc-4c39-b9f0-ad19cf79a3ca"/>
@@ -2129,17 +2143,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="247b3ed0-617a-4d1d-b8bd-a66944492619" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="334de605-b0fc-4c39-b9f0-ad19cf79a3ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2150,39 +2153,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF676F3C-E094-45CB-A3B9-969BA2EB17DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="334de605-b0fc-4c39-b9f0-ad19cf79a3ca"/>
-    <ds:schemaRef ds:uri="247b3ed0-617a-4d1d-b8bd-a66944492619"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20919586-F825-4328-A511-702B7F6D9530}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20919586-F825-4328-A511-702B7F6D9530}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="247b3ed0-617a-4d1d-b8bd-a66944492619"/>
-    <ds:schemaRef ds:uri="334de605-b0fc-4c39-b9f0-ad19cf79a3ca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF676F3C-E094-45CB-A3B9-969BA2EB17DD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74210780-D2ED-4E8B-8299-24F1A344B303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74210780-D2ED-4E8B-8299-24F1A344B303}"/>
 </file>
</xml_diff>